<commit_message>
YSSP: create 1048 OD pairs, test all work well, use distance for shortest path
</commit_message>
<xml_diff>
--- a/notebooks/scripts/city_sub_new_connected_edges_straight_line0617.xlsx
+++ b/notebooks/scripts/city_sub_new_connected_edges_straight_line0617.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1826,14 +1826,14 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>837</v>
+        <v>731</v>
       </c>
       <c r="B74" t="n">
-        <v>838</v>
+        <v>816</v>
       </c>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="n">
-        <v>15.30175205890257</v>
+        <v>338.0202213802057</v>
       </c>
       <c r="E74" t="n">
         <v>8.1</v>
@@ -1841,14 +1841,14 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>731</v>
+        <v>840</v>
       </c>
       <c r="B75" t="n">
-        <v>816</v>
+        <v>180</v>
       </c>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="n">
-        <v>338.0202213802057</v>
+        <v>363.9376157485787</v>
       </c>
       <c r="E75" t="n">
         <v>8.1</v>
@@ -1856,14 +1856,14 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>816</v>
+        <v>831</v>
       </c>
       <c r="B76" t="n">
-        <v>731</v>
+        <v>830</v>
       </c>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="n">
-        <v>338.0202213802057</v>
+        <v>22.22783221000168</v>
       </c>
       <c r="E76" t="n">
         <v>8.1</v>
@@ -1871,14 +1871,14 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>840</v>
+        <v>828</v>
       </c>
       <c r="B77" t="n">
-        <v>180</v>
+        <v>826</v>
       </c>
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="n">
-        <v>363.9376157485787</v>
+        <v>26.92042900992119</v>
       </c>
       <c r="E77" t="n">
         <v>8.1</v>
@@ -1886,14 +1886,14 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>180</v>
+        <v>828</v>
       </c>
       <c r="B78" t="n">
-        <v>840</v>
+        <v>825</v>
       </c>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="n">
-        <v>363.9376157485787</v>
+        <v>48.4794153554683</v>
       </c>
       <c r="E78" t="n">
         <v>8.1</v>
@@ -1901,14 +1901,14 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>831</v>
+        <v>826</v>
       </c>
       <c r="B79" t="n">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="n">
-        <v>22.22783221000168</v>
+        <v>21.60058442846288</v>
       </c>
       <c r="E79" t="n">
         <v>8.1</v>
@@ -1916,14 +1916,14 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>830</v>
+        <v>852</v>
       </c>
       <c r="B80" t="n">
-        <v>831</v>
+        <v>851</v>
       </c>
       <c r="C80" t="inlineStr"/>
       <c r="D80" t="n">
-        <v>22.22783221000168</v>
+        <v>13.26001334226355</v>
       </c>
       <c r="E80" t="n">
         <v>8.1</v>
@@ -1931,14 +1931,14 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>828</v>
+        <v>808</v>
       </c>
       <c r="B81" t="n">
-        <v>826</v>
+        <v>856</v>
       </c>
       <c r="C81" t="inlineStr"/>
       <c r="D81" t="n">
-        <v>26.92042900992119</v>
+        <v>45.55787836513344</v>
       </c>
       <c r="E81" t="n">
         <v>8.1</v>
@@ -1946,14 +1946,14 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>828</v>
+        <v>809</v>
       </c>
       <c r="B82" t="n">
-        <v>825</v>
+        <v>814</v>
       </c>
       <c r="C82" t="inlineStr"/>
       <c r="D82" t="n">
-        <v>48.4794153554683</v>
+        <v>28.21658262793809</v>
       </c>
       <c r="E82" t="n">
         <v>8.1</v>
@@ -1961,14 +1961,14 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>826</v>
+        <v>810</v>
       </c>
       <c r="B83" t="n">
-        <v>828</v>
+        <v>850</v>
       </c>
       <c r="C83" t="inlineStr"/>
       <c r="D83" t="n">
-        <v>26.92042900992119</v>
+        <v>20.28738866949541</v>
       </c>
       <c r="E83" t="n">
         <v>8.1</v>
@@ -1976,14 +1976,14 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>826</v>
+        <v>854</v>
       </c>
       <c r="B84" t="n">
-        <v>825</v>
+        <v>853</v>
       </c>
       <c r="C84" t="inlineStr"/>
       <c r="D84" t="n">
-        <v>21.60058442846288</v>
+        <v>20.34151055404855</v>
       </c>
       <c r="E84" t="n">
         <v>8.1</v>
@@ -1991,14 +1991,14 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>825</v>
+        <v>855</v>
       </c>
       <c r="B85" t="n">
-        <v>828</v>
+        <v>144</v>
       </c>
       <c r="C85" t="inlineStr"/>
       <c r="D85" t="n">
-        <v>48.4794153554683</v>
+        <v>42.61935863770476</v>
       </c>
       <c r="E85" t="n">
         <v>8.1</v>
@@ -2006,226 +2006,16 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>825</v>
+        <v>328</v>
       </c>
       <c r="B86" t="n">
-        <v>826</v>
+        <v>323</v>
       </c>
       <c r="C86" t="inlineStr"/>
       <c r="D86" t="n">
-        <v>21.60058442846288</v>
+        <v>29.06042896979379</v>
       </c>
       <c r="E86" t="n">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="n">
-        <v>852</v>
-      </c>
-      <c r="B87" t="n">
-        <v>851</v>
-      </c>
-      <c r="C87" t="inlineStr"/>
-      <c r="D87" t="n">
-        <v>13.26001334226355</v>
-      </c>
-      <c r="E87" t="n">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="n">
-        <v>851</v>
-      </c>
-      <c r="B88" t="n">
-        <v>852</v>
-      </c>
-      <c r="C88" t="inlineStr"/>
-      <c r="D88" t="n">
-        <v>13.26001334226355</v>
-      </c>
-      <c r="E88" t="n">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="n">
-        <v>808</v>
-      </c>
-      <c r="B89" t="n">
-        <v>856</v>
-      </c>
-      <c r="C89" t="inlineStr"/>
-      <c r="D89" t="n">
-        <v>45.55787836513344</v>
-      </c>
-      <c r="E89" t="n">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="n">
-        <v>856</v>
-      </c>
-      <c r="B90" t="n">
-        <v>808</v>
-      </c>
-      <c r="C90" t="inlineStr"/>
-      <c r="D90" t="n">
-        <v>45.55787836513344</v>
-      </c>
-      <c r="E90" t="n">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="n">
-        <v>809</v>
-      </c>
-      <c r="B91" t="n">
-        <v>814</v>
-      </c>
-      <c r="C91" t="inlineStr"/>
-      <c r="D91" t="n">
-        <v>28.21658262793809</v>
-      </c>
-      <c r="E91" t="n">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="n">
-        <v>814</v>
-      </c>
-      <c r="B92" t="n">
-        <v>809</v>
-      </c>
-      <c r="C92" t="inlineStr"/>
-      <c r="D92" t="n">
-        <v>28.21658262793809</v>
-      </c>
-      <c r="E92" t="n">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="n">
-        <v>810</v>
-      </c>
-      <c r="B93" t="n">
-        <v>850</v>
-      </c>
-      <c r="C93" t="inlineStr"/>
-      <c r="D93" t="n">
-        <v>20.28738866949541</v>
-      </c>
-      <c r="E93" t="n">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="n">
-        <v>850</v>
-      </c>
-      <c r="B94" t="n">
-        <v>810</v>
-      </c>
-      <c r="C94" t="inlineStr"/>
-      <c r="D94" t="n">
-        <v>20.28738866949541</v>
-      </c>
-      <c r="E94" t="n">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="n">
-        <v>854</v>
-      </c>
-      <c r="B95" t="n">
-        <v>853</v>
-      </c>
-      <c r="C95" t="inlineStr"/>
-      <c r="D95" t="n">
-        <v>20.34151055404855</v>
-      </c>
-      <c r="E95" t="n">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="n">
-        <v>853</v>
-      </c>
-      <c r="B96" t="n">
-        <v>854</v>
-      </c>
-      <c r="C96" t="inlineStr"/>
-      <c r="D96" t="n">
-        <v>20.34151055404855</v>
-      </c>
-      <c r="E96" t="n">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n">
-        <v>855</v>
-      </c>
-      <c r="B97" t="n">
-        <v>144</v>
-      </c>
-      <c r="C97" t="inlineStr"/>
-      <c r="D97" t="n">
-        <v>42.61935863770476</v>
-      </c>
-      <c r="E97" t="n">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="n">
-        <v>144</v>
-      </c>
-      <c r="B98" t="n">
-        <v>855</v>
-      </c>
-      <c r="C98" t="inlineStr"/>
-      <c r="D98" t="n">
-        <v>42.61935863770476</v>
-      </c>
-      <c r="E98" t="n">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="n">
-        <v>328</v>
-      </c>
-      <c r="B99" t="n">
-        <v>323</v>
-      </c>
-      <c r="C99" t="inlineStr"/>
-      <c r="D99" t="n">
-        <v>29.06042896979379</v>
-      </c>
-      <c r="E99" t="n">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="n">
-        <v>323</v>
-      </c>
-      <c r="B100" t="n">
-        <v>328</v>
-      </c>
-      <c r="C100" t="inlineStr"/>
-      <c r="D100" t="n">
-        <v>29.06042896979379</v>
-      </c>
-      <c r="E100" t="n">
         <v>8.1</v>
       </c>
     </row>

</xml_diff>